<commit_message>
CMO - fixing excel content
</commit_message>
<xml_diff>
--- a/JiraLoader/jiraLoader-core/src/test/resources/excelTestFiles/Import_JIRA_OK.xlsx
+++ b/JiraLoader/jiraLoader-core/src/test/resources/excelTestFiles/Import_JIRA_OK.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14730" windowHeight="6060"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16320" windowHeight="6990"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="4" r:id="rId1"/>
     <sheet name="Import" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -156,9 +157,6 @@
   </si>
   <si>
     <t>autoriser les mises à jours des tâches</t>
-  </si>
-  <si>
-    <t>Repercuter les mises à jours des tâches sur les sous taches</t>
   </si>
   <si>
     <t>Commentaires</t>
@@ -219,20 +217,23 @@
     <t>Rechercher si une story existe déjà lors de la creation</t>
   </si>
   <si>
+    <t xml:space="preserve">M5T_G01R12C06_BCA_KPSA_1048_1 | UO de test pour Jira </t>
+  </si>
+  <si>
+    <t>(true / false)</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Repercuter les mises à jours des sous-taches d'une tâche</t>
+  </si>
+  <si>
     <t>Lors de la création d'une story, le programme va rechercher si une story possède le même DEBUT de nom. 
-Par exemple, si la story porte le nom "M5T_G01R12C06_BCA_KPSA_1048_1 | nouveau SDM round robin - fichiers de conf osdp.cfg", le programme va rechercher si une story commence avec le nom "M5T_G01R12C06_BCA_KPSA_1048_1". Si oui, celle ci sera récupérer et aucune story ne sera créé</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M5T_G01R12C06_BCA_KPSA_1048_1 | UO de test pour Jira </t>
-  </si>
-  <si>
-    <t>(true / false)</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>true</t>
+Par exemple, si la story porte le nom "M5T_G01R12C06_BCA_KPSA_1048_1 | nouveau SDM round robin - fichiers de conf osdp.cfg", le programme va rechercher si une story commence avec le nom "M5T_G01R12C06_BCA_KPSA_1048_1". Si oui, celle ci sera récupérée et aucune story ne sera créée</t>
   </si>
 </sst>
 </file>
@@ -460,14 +461,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -475,9 +474,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,7 +783,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,24 +796,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="13" t="s">
+      <c r="F1" s="15"/>
+      <c r="G1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="13" t="s">
-        <v>48</v>
+      <c r="H1" s="16" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -845,16 +846,16 @@
         <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="14" t="s">
         <v>56</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -871,13 +872,13 @@
         <v>46</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>49</v>
+        <v>53</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -891,16 +892,16 @@
         <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>50</v>
+        <v>53</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -951,7 +952,7 @@
         <v>28</v>
       </c>
       <c r="C12" s="6"/>
-      <c r="E12" s="15"/>
+      <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
@@ -997,49 +998,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1072,7 +1073,7 @@
         <v>33</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Correction Commit précédent : - Modifications des autres fichiers excel pour la validation des tests
</commit_message>
<xml_diff>
--- a/JiraLoader/jiraLoader-core/src/test/resources/excelTestFiles/Import_JIRA_OK.xlsx
+++ b/JiraLoader/jiraLoader-core/src/test/resources/excelTestFiles/Import_JIRA_OK.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="16320" windowHeight="6990"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16320" windowHeight="6990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Configuration" sheetId="4" r:id="rId1"/>
     <sheet name="Import" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
   <si>
     <t>Version</t>
   </si>
@@ -234,6 +233,12 @@
   <si>
     <t>Lors de la création d'une story, le programme va rechercher si une story possède le même DEBUT de nom. 
 Par exemple, si la story porte le nom "M5T_G01R12C06_BCA_KPSA_1048_1 | nouveau SDM round robin - fichiers de conf osdp.cfg", le programme va rechercher si une story commence avec le nom "M5T_G01R12C06_BCA_KPSA_1048_1". Si oui, celle ci sera récupérée et aucune story ne sera créée</t>
+  </si>
+  <si>
+    <t>Référence Client</t>
+  </si>
+  <si>
+    <t>M5T_G01R12C06_BCA_KPSA_1048_1</t>
   </si>
 </sst>
 </file>
@@ -450,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -474,11 +479,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,7 +788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -796,23 +802,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="16" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>47</v>
       </c>
     </row>
@@ -979,9 +985,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -990,14 +996,15 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="74.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="46.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="29.28515625" customWidth="1"/>
+    <col min="6" max="6" width="74.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="46.28515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>8</v>
       </c>
@@ -1011,22 +1018,25 @@
         <v>0</v>
       </c>
       <c r="E1" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>40</v>
       </c>
@@ -1037,12 +1047,13 @@
       <c r="D2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="9"/>
+      <c r="E2" s="18"/>
       <c r="G2" s="9"/>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="9"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
@@ -1051,17 +1062,18 @@
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -1073,20 +1085,23 @@
         <v>33</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -1097,23 +1112,24 @@
       <c r="D5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
         <v>9</v>
@@ -1124,23 +1140,24 @@
       <c r="D6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1150,8 +1167,9 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1161,8 +1179,9 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1172,8 +1191,9 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1183,8 +1203,9 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1194,8 +1215,9 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1205,8 +1227,9 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1216,6 +1239,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C25" s="5"/>
@@ -1254,7 +1278,7 @@
           <x14:formula1>
             <xm:f>Configuration!$C$2:$C$14</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G1048576</xm:sqref>
+          <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>